<commit_message>
fix text for commontoolbox
</commit_message>
<xml_diff>
--- a/Projects/PEPSICOUK/Tests/Data/Inclusion_Exclusion_Template_Rollout.xlsx
+++ b/Projects/PEPSICOUK/Tests/Data/Inclusion_Exclusion_Template_Rollout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="exclusion_rules" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="47">
   <si>
     <t xml:space="preserve">KPI</t>
   </si>
@@ -36,6 +36,9 @@
     <t xml:space="preserve">Value</t>
   </si>
   <si>
+    <t xml:space="preserve">Ignore Store Policy</t>
+  </si>
+  <si>
     <t xml:space="preserve">All</t>
   </si>
   <si>
@@ -99,6 +102,9 @@
     <t xml:space="preserve">BLACK COUNTRY SNACKS, AKSAM PALUSZKI, LAJKONIK PALUSZKI, ALKA ELEPHANT, RUMPLERS, TABITHA, CHEF'S LARDER, BOROMIR, COFRESH, JIFFY POP, CROCO, THE CURATORS, FRESHERS, FUDCO, GEFEN, GINNI'S, OH MY GURU!, HALDIRAMS, HALDIRAMS SNACKS, INDIE BAY SNACKS, INNATE, JACK-LNK'S, EAZY-PP-PPCRN, ZWEIFEL CRISPS, HUNKY DORYS CRISPS, LAJKONIK JUNIOR, LOVE CHIN CHIN, NISHAS SNACKS, NUTELLA, OSEM SAVOURY SNACK, OUR LITTLE REBELL!ON, EPIC, CRAWFORDS, FLIPZ, OATIS, RYMUT SNACKS, GINCO, SUNSHINE SNACKS, JAY'S, MIDLAND SNACKS, RED MILL SAVOURY SNACKS, SENSIBLE PORTIONS, VISCONTI SNACKS, WELL &amp; TRULY SNACKS, WILD WEST, WILDING'S, BLUE DRAGON, BEPPS, BLUE DIAMOND, COFRESH SNACKS, SCHAR, OLD EL PASO, PLANTERS, LINWOODS, CYPRESSA, KOHINOOR SNACKS, KOIKEYA, PALUSZKI, LORENZ CRISPS, MCCOLGAN, ITSU, NAIRNS, NATURES STORE SNACKS, NIM'S, BAMBA SNACKS, BISSLI SNACKS, SHARWOODS, MR PORKY SNACKS, TYGRYSKI, THE REAL PORK CRACKLING CO SNACKS, THE SNAFFLING PIG CO, WHITWORTHS, YUM &amp; YAY</t>
   </si>
   <si>
+    <t xml:space="preserve">PRINGLES</t>
+  </si>
+  <si>
     <t xml:space="preserve">Price Scene</t>
   </si>
   <si>
@@ -114,6 +120,15 @@
     <t xml:space="preserve">Brand SOS of Segment</t>
   </si>
   <si>
+    <t xml:space="preserve">Some KPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PepsiCo Segment Space to Sales Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DORITOS</t>
+  </si>
+  <si>
     <t xml:space="preserve">additional_attribute_1</t>
   </si>
   <si>
@@ -130,9 +145,6 @@
   </si>
   <si>
     <t xml:space="preserve">Sub Brand Space to Sales Index</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PepsiCo Segment Space to Sales Index</t>
   </si>
   <si>
     <t xml:space="preserve">PepsiCo Sub Segment Space to Sales Index</t>
@@ -348,20 +360,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.5627530364373"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.8825910931174"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.71255060728745"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.3076923076923"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.7368421052632"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -378,299 +390,399 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -697,8 +809,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.2388663967611"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.5627530364373"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4939271255061"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
@@ -708,50 +820,50 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -770,16 +882,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.6356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.9554655870445"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="20.5668016194332"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.10526315789474"/>
   </cols>
@@ -789,54 +901,70 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>